<commit_message>
Adjusted .gitignore to ignore some temporary coding files. Improced get-data to use lineat interpolation to calculate missing information (where daily updates are missing and the data are static). Added helper functions for the linear interpolation
</commit_message>
<xml_diff>
--- a/data/raw_data.xlsx
+++ b/data/raw_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="291">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -860,6 +860,39 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240218174731/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.02.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240219021050/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.02.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240220031301/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.02.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.02.224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240221120805/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.02.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240222212239/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.02.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240223181530/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -869,7 +902,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -890,11 +923,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -939,16 +967,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -969,15 +993,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M134"/>
+  <dimension ref="A1:M139"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="690" topLeftCell="A114" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1230" topLeftCell="A113" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M134" activeCellId="0" sqref="M134"/>
+      <selection pane="bottomLeft" activeCell="M139" activeCellId="0" sqref="M139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5164,7 +5188,7 @@
       <c r="A120" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C120" s="0" t="n">
@@ -5205,7 +5229,7 @@
       <c r="A121" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C121" s="0" t="n">
@@ -5773,6 +5797,211 @@
       </c>
       <c r="M134" s="0" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>28775</v>
+      </c>
+      <c r="D135" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E135" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F135" s="0" t="n">
+        <v>68552</v>
+      </c>
+      <c r="G135" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H135" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I135" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J135" s="0" t="n">
+        <v>395</v>
+      </c>
+      <c r="K135" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="L135" s="0" t="n">
+        <v>4450</v>
+      </c>
+      <c r="M135" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>28775</v>
+      </c>
+      <c r="D136" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E136" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F136" s="0" t="n">
+        <v>68552</v>
+      </c>
+      <c r="G136" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H136" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I136" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J136" s="0" t="n">
+        <v>395</v>
+      </c>
+      <c r="K136" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="L136" s="0" t="n">
+        <v>4450</v>
+      </c>
+      <c r="M136" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>29313</v>
+      </c>
+      <c r="D137" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E137" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F137" s="0" t="n">
+        <v>69333</v>
+      </c>
+      <c r="G137" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H137" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I137" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J137" s="0" t="n">
+        <v>395</v>
+      </c>
+      <c r="K137" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="L137" s="0" t="n">
+        <v>4450</v>
+      </c>
+      <c r="M137" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>29313</v>
+      </c>
+      <c r="D138" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E138" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F138" s="0" t="n">
+        <v>69333</v>
+      </c>
+      <c r="G138" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H138" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I138" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J138" s="0" t="n">
+        <v>395</v>
+      </c>
+      <c r="K138" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="L138" s="0" t="n">
+        <v>4450</v>
+      </c>
+      <c r="M138" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>29313</v>
+      </c>
+      <c r="D139" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E139" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F139" s="0" t="n">
+        <v>69333</v>
+      </c>
+      <c r="G139" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H139" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I139" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J139" s="0" t="n">
+        <v>395</v>
+      </c>
+      <c r="K139" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="L139" s="0" t="n">
+        <v>4450</v>
+      </c>
+      <c r="M139" s="0" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>